<commit_message>
Add tests for simple2.xlsx
</commit_message>
<xml_diff>
--- a/X2tConverter/test/ExampleFiles/xlsb2xlsx/simple2.xlsx
+++ b/X2tConverter/test/ExampleFiles/xlsb2xlsx/simple2.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="0" dateCompatibility="1" hidePivotFieldList="0" showPivotChartFilter="0" updateLinks="always"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <workbookPr allowRefreshQuery="0" autoCompressPictures="1" backupFile="0" checkCompatibility="0" codeName="0" date1904="0" dateCompatibility="1" defaultThemeVersion="0" filterPrivacy="0" hidePivotFieldList="0" promptedSolutions="0" publishItems="0" refreshAllConnections="0" showBorderUnselectedTables="0" showInkAnnotation="1" showObjects="all" showPivotChartFilter="0" updateLinks="always"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Лист2" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Slicer_it">#N/A</definedName>
   </definedNames>
   <calcPr calcId="0" calcMode="autoNoTable" fullCalcOnLoad="0" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001" fullPrecision="1" calcCompleted="0" calcOnSave="1" concurrentCalc="1" concurrentManualCount="1" forceFullCalc="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
-      <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicerCache r:id="rId1">
-</x14:slicerCache>
+    <ext uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
+      <x15:slicerCaches>
+        <x14:slicerCache r:id="rId4"/>
       </x15:slicerCaches>
     </ext>
   </extLst>
@@ -30,25 +32,11 @@
     <author>tc={5A175D1A-2D6E-3CC8-2227-22732FCB5686}</author>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0" xr:uid="{5A175D1A-2D6E-3CC8-2227-22732FCB5686}">
+    <comment ref="D4" authorId="0" xr:uid="{00000000-0000-0000-0000-000000000000}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Vik:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">
+        <t xml:space="preserve">Vik:
 test comment
 </t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -84,45 +72,63 @@
     <font>
       <i val="0"/>
       <strike val="0"/>
+      <condense val="0"/>
+      <extend val="0"/>
+      <outline val="0"/>
+      <shadow val="0"/>
       <u val="none"/>
       <vertAlign val="baseline"/>
       <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <i val="0"/>
       <strike val="0"/>
+      <condense val="0"/>
+      <extend val="0"/>
+      <outline val="0"/>
+      <shadow val="0"/>
       <u val="none"/>
       <vertAlign val="baseline"/>
       <sz val="9.000000"/>
       <color auto="1"/>
       <name val="Tahoma"/>
+      <family val="0"/>
+      <charset val="0"/>
       <scheme val="none"/>
     </font>
     <font>
       <i val="0"/>
       <strike val="0"/>
+      <condense val="0"/>
+      <extend val="0"/>
+      <outline val="0"/>
+      <shadow val="0"/>
       <u val="none"/>
       <vertAlign val="baseline"/>
       <sz val="9.000000"/>
       <color auto="1"/>
       <name val="Tahoma"/>
+      <family val="0"/>
+      <charset val="0"/>
       <scheme val="none"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none">
-        <fgColor/>
+        <fgColor indexed="64"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="gray125">
-        <fgColor/>
+        <fgColor indexed="64"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -148,23 +154,21 @@
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" quotePrefix="0" pivotButton="0">
-      <alignment horizontal="general" indent="0" relativeIndent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" relativeIndent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
       <protection hidden="0" locked="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" quotePrefix="0" pivotButton="0">
-      <alignment horizontal="general" indent="0" relativeIndent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" relativeIndent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
       <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+    <ext uri="{EB79DEF2-80B8-43E5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
@@ -246,14 +250,70 @@
 </personList>
 </file>
 
-<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_it" sourceName="it">
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" r:id="rId1" refreshedDateIso="0.000000" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="2">
+  <cacheSource connectionId="0" type="worksheet">
+    <worksheetSource sheet="Лист1" ref="C6:D8"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="1" mappingCount="0" numFmtId="-1">
+      <sharedItems count="0" containsBlank="0" containsDate="0" containsInteger="1" containsMixedTypes="0" containsNonDate="1" containsNumber="1" containsSemiMixedTypes="0" containsString="0" longText="0" minValue="8" maxValue="178"/>
+    </cacheField>
+    <cacheField name="4" mappingCount="0" numFmtId="-1">
+      <sharedItems count="0" containsBlank="0" containsDate="0" containsInteger="1" containsMixedTypes="0" containsNonDate="1" containsNumber="1" containsSemiMixedTypes="0" containsString="0" longText="0" minValue="9" maxValue="87"/>
+    </cacheField>
+  </cacheFields>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
-      <x15:tableSlicerCache tableId="1" column="1" sortOrder="ascending" customListSort="1" crossFilter="showItemsWithDataAtTop"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition pivotCacheId="0"/>
     </ext>
   </extLst>
-</slicerCacheDefinition>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" count="2">
+  <r>
+    <n v="8"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <n v="178"/>
+    <n v="87"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="PivotTable1" cacheId="0" dataCaption="Значения" applyAlignmentFormats="0" applyBorderFormats="0" applyFontFormats="0" applyNumberFormats="0" applyPatternFormats="0" applyWidthHeightFormats="1" autoFormatId="1" createdVersion="4" immersive="0" indent="0" itemPrintTitles="1" minRefreshableVersion="3" multipleFieldFilters="0" outline="1" outlineData="1" updatedVersion="4" useAutoFormatting="1" visualTotals="0">
+  <location colPageCount="0" firstDataCol="0" firstDataRow="2" firstHeaderRow="1" ref="A3:B5" rowPageCount="0"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" dataSourceSort="0" includeNewItemsInFilter="1" showAll="0" axis="axisValues" sortType="manual" numFmtId="0"/>
+    <pivotField dataField="1" dataSourceSort="0" includeNewItemsInFilter="1" showAll="0" axis="axisValues" sortType="manual" numFmtId="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i i="0" r="0" t="data"/>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i i="0" r="0" t="data">
+      <x v="0"/>
+    </i>
+    <i i="1" r="0" t="data">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of 1" baseField="0" baseItem="0" fld="0" numFmtId="0"/>
+    <dataField name="Sum of 4" baseField="0" baseItem="0" fld="1" numFmtId="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showColHeaders="1" showColStripes="0" showLastColumn="1" showRowHeaders="1" showRowStripes="0"/>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?><slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x xr10" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" name="Slicer_it" sourceName="it"><extLst><ext uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}"><x15:tableSlicerCache tableId="1" column="1" sortOrder="ascending" customListSort="1" crossFilter="showItemsWithDataAtTop"></x15:tableSlicerCache></ext></extLst></slicerCacheDefinition>
 </file>
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -273,289 +333,6 @@
 </table>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -564,7 +341,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="000000"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -780,6 +557,53 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
+    <sheetView windowProtection="0" showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" showWhiteSpace="0" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col bestFit="1" collapsed="0" customWidth="0" hidden="0" min="1" max="1" outlineLevel="0" phonetic="0" style="0" width="9.36328125"/>
+    <col bestFit="1" collapsed="0" customWidth="0" hidden="0" min="2" max="2" outlineLevel="0" phonetic="0" style="0" width="8.54296875"/>
+  </cols>
+  <sheetData>
+    <row r="3" ht="14.5">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" ht="14.5">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" ht="14.5">
+      <c r="A5">
+        <v>186</v>
+      </c>
+      <c r="B5">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection password="0" autoFilter="0" content="1" deleteColumns="0" deleteRows="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertHyperlinks="0" insertRows="0" objects="1" pivotTables="0" scenarios="1" selectLockedCells="1" selectUnlockedCells="1" sheet="0" sort="0"/>
+  <printOptions headings="0" gridLines="0" gridLinesSet="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1" r:id=""/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr syncHorizontal="0" syncVertical="0" transitionEvaluation="0" transitionEntry="0" published="1" filterMode="0" enableFormatConditionsCalculation="0">
+    <tabColor auto="1"/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
+  <sheetViews>
     <sheetView windowProtection="0" showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" showWhiteSpace="0" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -848,66 +672,19 @@
   </sheetData>
   <sheetProtection password="0" autoFilter="0" content="1" deleteColumns="0" deleteRows="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertHyperlinks="0" insertRows="0" objects="1" pivotTables="0" scenarios="1" selectLockedCells="1" selectUnlockedCells="1" sheet="0" sort="0"/>
   <printOptions headings="0" gridLines="0" gridLinesSet="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700776" bottom="0.75196850393700776" header="0.29999999999999993" footer="0.29999999999999993"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1" r:id=""/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+    <ext uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
       <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicer r:id="rId6"/>
+        <x14:slicer r:id="rId5"/>
       </x14:slicerList>
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr syncHorizontal="0" syncVertical="0" transitionEvaluation="0" transitionEntry="0" published="1" filterMode="0" enableFormatConditionsCalculation="0">
-    <tabColor auto="1"/>
-    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView windowProtection="0" showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" showWhiteSpace="0" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col bestFit="1" collapsed="0" customWidth="0" hidden="0" min="1" max="1" outlineLevel="0" style="0" width="9.36328125"/>
-    <col bestFit="1" collapsed="0" customWidth="0" hidden="0" min="2" max="2" outlineLevel="0" style="0" width="8.54296875"/>
-  </cols>
-  <sheetData>
-    <row r="3" ht="14.5">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" ht="14.5">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" ht="14.5">
-      <c r="A5">
-        <v>186</v>
-      </c>
-      <c r="B5">
-        <v>96</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection password="0" autoFilter="0" content="1" deleteColumns="0" deleteRows="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertHyperlinks="0" insertRows="0" objects="1" pivotTables="0" scenarios="1" selectLockedCells="1" selectUnlockedCells="1" sheet="0" sort="0"/>
-  <printOptions headings="0" gridLines="0" gridLinesSet="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700776" bottom="0.75196850393700776" header="0.29999999999999993" footer="0.29999999999999993"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-</worksheet>
 </file>
</xml_diff>